<commit_message>
formato y unas cositas
</commit_message>
<xml_diff>
--- a/Barbie_Financiera_FASE_2/BF-0044/BF-0044 Escenarios y Casos de Prueba.xlsx
+++ b/Barbie_Financiera_FASE_2/BF-0044/BF-0044 Escenarios y Casos de Prueba.xlsx
@@ -5,23 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esenedusv-my.sharepoint.com/personal/20235662_esen_edu_sv/Documents/Ciclo 03-2/agile/Proyecto/Proyecto-PDS-BarbieFinanciera/FASE 2/BF-0044/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esenedusv-my.sharepoint.com/personal/20235662_esen_edu_sv/Documents/Ciclo 03-2/agile/Proyecto/Proyecto-PDS-BarbieFinanciera/Barbie_Financiera_FASE_2/BF-0044/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="8_{2E566EB6-A64A-4FA2-A4D8-D505CE2FB55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F796FFEB-2F7A-4C6D-BAF6-A33C2CACD87D}"/>
+  <xr:revisionPtr revIDLastSave="443" documentId="8_{2E566EB6-A64A-4FA2-A4D8-D505CE2FB55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16C36958-FF94-4FD5-AF36-7DD689A7EE73}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escenarios" sheetId="2" r:id="rId1"/>
     <sheet name="Casos de Prueba" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>Criterios de Aceptación</t>
   </si>
@@ -214,6 +227,12 @@
   </si>
   <si>
     <t>Los reportes tanto de la función "Detalle de Categorías" como de "Balance" son actualizados al agregar un nuevo gasto.</t>
+  </si>
+  <si>
+    <t>Defecto</t>
+  </si>
+  <si>
+    <t>Caso de prueba no ha sido implementado en la aplicación.</t>
   </si>
 </sst>
 </file>
@@ -364,18 +383,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="2" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -559,13 +578,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="20"/>
+      </left>
+      <right style="thin">
+        <color indexed="20"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -620,17 +728,53 @@
     <xf numFmtId="49" fontId="8" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -656,56 +800,38 @@
     <xf numFmtId="49" fontId="10" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1865,29 +1991,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.2" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.8" customHeight="1">
-      <c r="A2" s="26">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="38">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="40" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -1895,25 +2021,25 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="31.2" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="29"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27.6" customHeight="1">
-      <c r="A4" s="44">
+      <c r="A4" s="32">
         <v>2</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="28">
         <v>2</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="15" t="s">
@@ -1921,25 +2047,25 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.2" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="39"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30.6" customHeight="1">
-      <c r="A6" s="34">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="20">
         <v>3</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="18" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -1947,10 +2073,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="31.8" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="31"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="16" t="s">
         <v>25</v>
       </c>
@@ -1974,6 +2100,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="A6:A7"/>
@@ -1982,12 +2114,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2002,13 +2128,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="139" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.95" customHeight="1"/>
@@ -2022,7 +2148,7 @@
     <col min="10" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2047,8 +2173,11 @@
       <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="42" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="89.4" customHeight="1">
+    <row r="2" spans="1:9" ht="89.4" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2070,11 +2199,12 @@
       <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="43" t="s">
         <v>11</v>
       </c>
+      <c r="I2" s="49"/>
     </row>
-    <row r="3" spans="1:8" ht="147" customHeight="1">
+    <row r="3" spans="1:9" ht="147" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -2096,11 +2226,12 @@
       <c r="G3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="48" t="s">
         <v>11</v>
       </c>
+      <c r="I3" s="50"/>
     </row>
-    <row r="4" spans="1:8" ht="98.4" customHeight="1">
+    <row r="4" spans="1:9" ht="98.4" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -2122,11 +2253,14 @@
       <c r="G4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="47" t="s">
         <v>38</v>
       </c>
+      <c r="I4" s="51" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="78.150000000000006" customHeight="1">
+    <row r="5" spans="1:9" ht="78.150000000000006" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
@@ -2148,11 +2282,14 @@
       <c r="G5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="45" t="s">
         <v>38</v>
       </c>
+      <c r="I5" s="51" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="85.8" customHeight="1">
+    <row r="6" spans="1:9" ht="85.8" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -2174,11 +2311,12 @@
       <c r="G6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="46" t="s">
         <v>11</v>
       </c>
+      <c r="I6" s="52"/>
     </row>
-    <row r="7" spans="1:8" ht="78.150000000000006" customHeight="1">
+    <row r="7" spans="1:9" ht="78.150000000000006" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
@@ -2200,11 +2338,12 @@
       <c r="G7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="46" t="s">
         <v>11</v>
       </c>
+      <c r="I7" s="51"/>
     </row>
-    <row r="8" spans="1:8" ht="91.8" customHeight="1">
+    <row r="8" spans="1:9" ht="91.8" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
@@ -2226,9 +2365,15 @@
       <c r="G8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="45" t="s">
         <v>38</v>
       </c>
+      <c r="I8" s="51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13.95" customHeight="1">
+      <c r="F11" s="44"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>